<commit_message>
Updated Vendor Management Create CompanyVendor
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_UAE_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_UAE_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="138" activeTab="141"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="140" activeTab="141"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6177" uniqueCount="1813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6181" uniqueCount="1813">
   <si>
     <t>Description</t>
   </si>
@@ -5609,7 +5609,7 @@
     <t>1009128</t>
   </si>
   <si>
-    <t>GlobalCompanyVendor</t>
+    <t>24TTL Digital Marketing Solutions DMCC</t>
   </si>
 </sst>
 </file>
@@ -13494,10 +13494,10 @@
 
 <file path=xl/worksheets/sheet142.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13701,6 +13701,26 @@
       </c>
       <c r="D14" s="102" t="s">
         <v>871</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="104" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B15" s="104"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="17" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="104" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B16" s="104"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="105" t="s">
+        <v>1672</v>
       </c>
     </row>
   </sheetData>
@@ -14258,7 +14278,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A29" sqref="A29:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15925,7 +15945,7 @@
   <dimension ref="A1:FJ154"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Latest Data sheets
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_UAE_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_UAE_REGRESSION.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\OneDrive - Cognizant\Documents\WPP Global TestScripts\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestSuite\branches\bau_environment\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E85F19-10CD-4643-9260-F34F0813B2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="145" activeTab="147"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="142" activeTab="145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -171,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6230" uniqueCount="1858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6238" uniqueCount="1859">
   <si>
     <t>Description</t>
   </si>
@@ -5587,9 +5588,6 @@
     <t>Zip Code</t>
   </si>
   <si>
-    <t>05/30/2021</t>
-  </si>
-  <si>
     <t>BB011111</t>
   </si>
   <si>
@@ -5747,12 +5745,18 @@
   </si>
   <si>
     <t>79,809.63</t>
+  </si>
+  <si>
+    <t>10/30/2021</t>
+  </si>
+  <si>
+    <t>2128_GlobalVendor 16August2021 20:41:14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6263,7 +6267,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6540,14 +6544,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6619,8 +6623,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -6628,7 +6632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6759,7 +6763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6300-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6847,7 +6851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6400-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -7103,7 +7107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6500-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7155,7 +7159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6600-000000000000}">
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7349,7 +7353,7 @@
 </file>
 
 <file path=xl/worksheets/sheet104.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6700-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7405,7 +7409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet105.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7454,7 +7458,7 @@
 </file>
 
 <file path=xl/worksheets/sheet106.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6900-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7516,7 +7520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet107.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6A00-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -7906,7 +7910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet108.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6B00-000000000000}">
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -8082,11 +8086,11 @@
 </file>
 
 <file path=xl/worksheets/sheet109.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6C00-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8205,7 +8209,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8349,7 +8353,7 @@
 </file>
 
 <file path=xl/worksheets/sheet110.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6D00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8453,7 +8457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet111.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6E00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8505,7 +8509,7 @@
 </file>
 
 <file path=xl/worksheets/sheet112.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6F00-000000000000}">
   <dimension ref="A1:BO8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9572,7 +9576,7 @@
 </file>
 
 <file path=xl/worksheets/sheet113.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9648,7 +9652,7 @@
 </file>
 
 <file path=xl/worksheets/sheet114.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9727,7 +9731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet115.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7200-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9867,7 +9871,7 @@
 </file>
 
 <file path=xl/worksheets/sheet116.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7300-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9918,7 +9922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet117.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7400-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10056,7 +10060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet118.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7500-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10170,7 +10174,7 @@
 </file>
 
 <file path=xl/worksheets/sheet119.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7600-000000000000}">
   <dimension ref="A1:BI4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10544,7 +10548,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10694,7 +10698,7 @@
 </file>
 
 <file path=xl/worksheets/sheet120.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7700-000000000000}">
   <dimension ref="A1:BI4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11067,7 +11071,7 @@
 </file>
 
 <file path=xl/worksheets/sheet121.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7800-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11140,7 +11144,7 @@
 </file>
 
 <file path=xl/worksheets/sheet122.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7900-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11252,7 +11256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet123.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7A00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11298,7 +11302,7 @@
 </file>
 
 <file path=xl/worksheets/sheet124.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7B00-000000000000}">
   <dimension ref="A1:BO2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11720,7 +11724,7 @@
 </file>
 
 <file path=xl/worksheets/sheet125.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7C00-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11907,8 +11911,8 @@
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1"/>
-    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{00000000-0004-0000-7C00-000000000000}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-7C00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -11916,7 +11920,7 @@
 </file>
 
 <file path=xl/worksheets/sheet126.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7D00-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12078,8 +12082,8 @@
     <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
-    <hyperlink ref="C9" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-7D00-000000000000}"/>
+    <hyperlink ref="C9" r:id="rId2" xr:uid="{00000000-0004-0000-7D00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -12087,8 +12091,8 @@
 </file>
 
 <file path=xl/worksheets/sheet127.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7E00-000000000000}">
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -12098,9 +12102,7 @@
   <cols>
     <col min="1" max="1" width="19.5703125" style="102" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="30.7109375" style="102" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.140625" style="102" collapsed="1"/>
-    <col min="5" max="7" width="9.140625" style="102"/>
-    <col min="8" max="16384" width="9.140625" style="102" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="102" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -12122,10 +12124,10 @@
         <v>49</v>
       </c>
       <c r="B2" s="102" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>1809</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1810</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -12133,13 +12135,13 @@
         <v>658</v>
       </c>
       <c r="B3" s="105" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C3" s="105" t="s">
         <v>1825</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="D3" s="102" t="s">
         <v>1826</v>
-      </c>
-      <c r="D3" s="102" t="s">
-        <v>1827</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -12147,13 +12149,13 @@
         <v>820</v>
       </c>
       <c r="B4" s="105" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C4" s="102" t="s">
         <v>1828</v>
       </c>
-      <c r="C4" s="102" t="s">
+      <c r="D4" s="102" t="s">
         <v>1829</v>
-      </c>
-      <c r="D4" s="102" t="s">
-        <v>1830</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -12167,7 +12169,7 @@
         <v>611</v>
       </c>
       <c r="D5" s="102" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -12175,13 +12177,13 @@
         <v>1164</v>
       </c>
       <c r="B6" s="105" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C6" s="105" t="s">
         <v>1815</v>
       </c>
-      <c r="C6" s="105" t="s">
-        <v>1816</v>
-      </c>
       <c r="D6" s="102" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -12195,7 +12197,7 @@
         <v>871</v>
       </c>
       <c r="D7" s="102" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -12203,13 +12205,13 @@
         <v>870</v>
       </c>
       <c r="B8" s="102" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C8" s="102" t="s">
         <v>1817</v>
       </c>
-      <c r="C8" s="102" t="s">
-        <v>1818</v>
-      </c>
       <c r="D8" s="102" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -12217,10 +12219,10 @@
         <v>26</v>
       </c>
       <c r="B9" s="76" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C9" s="76" t="s">
         <v>1819</v>
-      </c>
-      <c r="C9" s="76" t="s">
-        <v>1820</v>
       </c>
       <c r="D9" s="102" t="s">
         <v>215</v>
@@ -12231,10 +12233,10 @@
         <v>1165</v>
       </c>
       <c r="B10" s="105" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C10" s="105" t="s">
         <v>1821</v>
-      </c>
-      <c r="C10" s="105" t="s">
-        <v>1822</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -12264,10 +12266,10 @@
         <v>1168</v>
       </c>
       <c r="B13" s="102" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C13" s="102" t="s">
         <v>1823</v>
-      </c>
-      <c r="C13" s="102" t="s">
-        <v>1824</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -12310,8 +12312,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
-    <hyperlink ref="C9" r:id="rId2" display="2113Auto01@oglivy.com"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-7E00-000000000000}"/>
+    <hyperlink ref="C9" r:id="rId2" display="2113Auto01@oglivy.com" xr:uid="{00000000-0004-0000-7E00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -12319,8 +12321,8 @@
 </file>
 
 <file path=xl/worksheets/sheet128.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7F00-000000000000}">
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -12330,8 +12332,7 @@
   <cols>
     <col min="1" max="1" width="19.5703125" style="102" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="30.7109375" style="102" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="9.140625" style="102"/>
-    <col min="6" max="16384" width="9.140625" style="102" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="102" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -12350,10 +12351,10 @@
         <v>49</v>
       </c>
       <c r="B2" s="102" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>1809</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1810</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -12367,10 +12368,10 @@
         <v>659</v>
       </c>
       <c r="B4" s="105" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C4" s="105" t="s">
         <v>1835</v>
-      </c>
-      <c r="C4" s="105" t="s">
-        <v>1836</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -12384,10 +12385,10 @@
         <v>660</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="C6" s="102" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -12406,10 +12407,10 @@
         <v>1164</v>
       </c>
       <c r="B8" s="105" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C8" s="105" t="s">
         <v>1815</v>
-      </c>
-      <c r="C8" s="105" t="s">
-        <v>1816</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -12428,10 +12429,10 @@
         <v>870</v>
       </c>
       <c r="B10" s="102" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C10" s="102" t="s">
         <v>1817</v>
-      </c>
-      <c r="C10" s="102" t="s">
-        <v>1818</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -12439,10 +12440,10 @@
         <v>26</v>
       </c>
       <c r="B11" s="76" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C11" s="76" t="s">
         <v>1819</v>
-      </c>
-      <c r="C11" s="76" t="s">
-        <v>1820</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -12450,10 +12451,10 @@
         <v>1165</v>
       </c>
       <c r="B12" s="105" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C12" s="105" t="s">
         <v>1821</v>
-      </c>
-      <c r="C12" s="105" t="s">
-        <v>1822</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -12483,10 +12484,10 @@
         <v>1168</v>
       </c>
       <c r="B15" s="102" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C15" s="102" t="s">
         <v>1823</v>
-      </c>
-      <c r="C15" s="102" t="s">
-        <v>1824</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -12529,8 +12530,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="C11" r:id="rId2" display="2113Auto01@oglivy.com"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-7F00-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId2" display="2113Auto01@oglivy.com" xr:uid="{00000000-0004-0000-7F00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -12538,8 +12539,8 @@
 </file>
 
 <file path=xl/worksheets/sheet129.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8000-000000000000}">
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -12550,8 +12551,7 @@
     <col min="1" max="1" width="19.5703125" style="102" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.7109375" style="102" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="38.28515625" style="102" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="9.140625" style="102"/>
-    <col min="6" max="16384" width="9.140625" style="102" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="102" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -12570,10 +12570,10 @@
         <v>49</v>
       </c>
       <c r="B2" s="102" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>1809</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1810</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -12587,10 +12587,10 @@
         <v>1171</v>
       </c>
       <c r="B4" s="105" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C4" s="105" t="s">
         <v>1811</v>
-      </c>
-      <c r="C4" s="105" t="s">
-        <v>1812</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -12604,10 +12604,10 @@
         <v>1162</v>
       </c>
       <c r="B6" s="105" t="s">
+        <v>1812</v>
+      </c>
+      <c r="C6" s="102" t="s">
         <v>1813</v>
-      </c>
-      <c r="C6" s="102" t="s">
-        <v>1814</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -12626,10 +12626,10 @@
         <v>1164</v>
       </c>
       <c r="B8" s="105" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C8" s="105" t="s">
         <v>1815</v>
-      </c>
-      <c r="C8" s="105" t="s">
-        <v>1816</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -12648,10 +12648,10 @@
         <v>870</v>
       </c>
       <c r="B10" s="102" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C10" s="102" t="s">
         <v>1817</v>
-      </c>
-      <c r="C10" s="102" t="s">
-        <v>1818</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -12659,10 +12659,10 @@
         <v>26</v>
       </c>
       <c r="B11" s="76" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C11" s="76" t="s">
         <v>1819</v>
-      </c>
-      <c r="C11" s="76" t="s">
-        <v>1820</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -12670,10 +12670,10 @@
         <v>1165</v>
       </c>
       <c r="B12" s="105" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C12" s="105" t="s">
         <v>1821</v>
-      </c>
-      <c r="C12" s="105" t="s">
-        <v>1822</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -12703,10 +12703,10 @@
         <v>1168</v>
       </c>
       <c r="B15" s="102" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C15" s="102" t="s">
         <v>1823</v>
-      </c>
-      <c r="C15" s="102" t="s">
-        <v>1824</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -12749,8 +12749,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="C11" r:id="rId2" display="2113Auto01@oglivy.com"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-8000-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId2" display="2113Auto01@oglivy.com" xr:uid="{00000000-0004-0000-8000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -12758,7 +12758,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12799,7 +12799,7 @@
 </file>
 
 <file path=xl/worksheets/sheet130.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12867,7 +12867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet131.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12947,7 +12947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet132.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13027,7 +13027,7 @@
 </file>
 
 <file path=xl/worksheets/sheet133.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8400-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13110,7 +13110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet134.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8500-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13210,8 +13210,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="C10" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-8500-000000000000}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{00000000-0004-0000-8500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -13219,7 +13219,7 @@
 </file>
 
 <file path=xl/worksheets/sheet135.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8600-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13319,8 +13319,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="C10" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-8600-000000000000}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{00000000-0004-0000-8600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -13328,7 +13328,7 @@
 </file>
 
 <file path=xl/worksheets/sheet136.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8700-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13388,7 +13388,7 @@
 </file>
 
 <file path=xl/worksheets/sheet137.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8800-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13448,7 +13448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet138.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8900-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13497,7 +13497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet139.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8A00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13557,7 +13557,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13598,7 +13598,7 @@
 </file>
 
 <file path=xl/worksheets/sheet140.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8B00-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -13661,7 +13661,7 @@
 </file>
 
 <file path=xl/worksheets/sheet141.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8C00-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -13711,11 +13711,11 @@
 </file>
 
 <file path=xl/worksheets/sheet142.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8D00-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13876,7 +13876,7 @@
         <v>1184</v>
       </c>
       <c r="D11" s="102" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -13928,7 +13928,7 @@
       <c r="B15" s="104"/>
       <c r="C15" s="104"/>
       <c r="D15" s="17" t="s">
-        <v>1804</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -13943,9 +13943,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-8D00-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-8D00-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-8D00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -13953,11 +13953,11 @@
 </file>
 
 <file path=xl/worksheets/sheet143.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8E00-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14042,14 +14042,14 @@
         <v>79</v>
       </c>
       <c r="D6" s="102" t="s">
-        <v>79</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-8E00-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-8E00-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-8E00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -14057,11 +14057,11 @@
 </file>
 
 <file path=xl/worksheets/sheet144.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8F00-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14071,7 +14071,7 @@
     <col min="4" max="16384" width="9.140625" style="102" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>181</v>
       </c>
@@ -14081,15 +14081,18 @@
       <c r="C1" s="102">
         <v>1221</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="102">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
         <v>164</v>
       </c>
       <c r="B2" s="106"/>
       <c r="C2" s="106"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="102" t="s">
         <v>26</v>
       </c>
@@ -14099,8 +14102,11 @@
       <c r="C3" s="76" t="s">
         <v>1178</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="76" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="102" t="s">
         <v>836</v>
       </c>
@@ -14110,8 +14116,11 @@
       <c r="C4" s="102">
         <v>958647231</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="102">
+        <v>958647231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="102" t="s">
         <v>1177</v>
       </c>
@@ -14121,23 +14130,27 @@
       <c r="C5" s="102" t="s">
         <v>79</v>
       </c>
+      <c r="D5" s="102" t="s">
+        <v>611</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-8F00-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-8F00-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{72504A4E-A5D4-48C6-9A96-5435C4E345F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet145.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-9000-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14147,7 +14160,7 @@
     <col min="3" max="16384" width="9.140625" style="102" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>181</v>
       </c>
@@ -14157,13 +14170,16 @@
       <c r="C1" s="102">
         <v>1221</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="102">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="102" t="s">
         <v>178</v>
       </c>
@@ -14172,6 +14188,9 @@
       </c>
       <c r="C3" s="102" t="s">
         <v>79</v>
+      </c>
+      <c r="D3" s="102" t="s">
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -14181,11 +14200,11 @@
 </file>
 
 <file path=xl/worksheets/sheet146.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-9100-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14195,7 +14214,7 @@
     <col min="3" max="16384" width="9.140625" style="102" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>181</v>
       </c>
@@ -14205,14 +14224,17 @@
       <c r="C1" s="102">
         <v>1221</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="102">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
         <v>1182</v>
       </c>
       <c r="B2" s="106"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="102" t="s">
         <v>178</v>
       </c>
@@ -14221,6 +14243,9 @@
       </c>
       <c r="C3" s="102" t="s">
         <v>79</v>
+      </c>
+      <c r="D3" s="102" t="s">
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -14230,7 +14255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet147.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-9200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14254,27 +14279,27 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="B2" s="105"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="102" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="B3" s="105"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="102" t="s">
+        <v>1839</v>
+      </c>
+      <c r="B4" s="105" t="s">
         <v>1840</v>
-      </c>
-      <c r="B4" s="105" t="s">
-        <v>1841</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="102" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="B5" s="102">
         <v>1221002</v>
@@ -14282,14 +14307,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet148.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-9300-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -14303,31 +14329,31 @@
         <v>1000</v>
       </c>
       <c r="B1" s="102" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C1" s="102" t="s">
         <v>1843</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="D1" s="102" t="s">
         <v>1844</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="E1" s="102" t="s">
         <v>1845</v>
       </c>
-      <c r="E1" s="102" t="s">
+      <c r="F1" s="102" t="s">
         <v>1846</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="G1" s="102" t="s">
         <v>1847</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="H1" s="102" t="s">
         <v>1848</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="I1" s="102" t="s">
         <v>1849</v>
       </c>
-      <c r="I1" s="102" t="s">
+      <c r="J1" s="102" t="s">
         <v>1850</v>
-      </c>
-      <c r="J1" s="102" t="s">
-        <v>1851</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -14335,28 +14361,28 @@
         <v>1221</v>
       </c>
       <c r="B2" s="102" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C2" s="102" t="s">
         <v>1852</v>
       </c>
-      <c r="C2" s="102" t="s">
+      <c r="D2" s="102" t="s">
         <v>1853</v>
       </c>
-      <c r="D2" s="102" t="s">
+      <c r="E2" s="102" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F2" s="102" t="s">
         <v>1854</v>
       </c>
-      <c r="E2" s="102" t="s">
-        <v>1841</v>
-      </c>
-      <c r="F2" s="102" t="s">
+      <c r="G2" s="102" t="s">
         <v>1855</v>
-      </c>
-      <c r="G2" s="102" t="s">
-        <v>1856</v>
       </c>
       <c r="H2" s="102" t="s">
         <v>996</v>
       </c>
       <c r="I2" s="102" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="J2" s="102" t="s">
         <v>1493</v>
@@ -14364,11 +14390,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -14619,7 +14646,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1"/>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -14627,14 +14654,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:G30"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14899,7 +14926,7 @@
         <v>1526</v>
       </c>
       <c r="G11" s="105" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -14922,7 +14949,7 @@
         <v>1526</v>
       </c>
       <c r="G12" s="105" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -15298,7 +15325,7 @@
         <v>1795</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>1804</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -15311,12 +15338,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5"/>
-    <hyperlink ref="G4" r:id="rId6"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0F00-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0F00-000003000000}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0F00-000004000000}"/>
+    <hyperlink ref="G4" r:id="rId6" xr:uid="{00000000-0004-0000-0F00-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -15324,7 +15351,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -15694,7 +15721,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -16014,7 +16041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -16294,60 +16321,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:FJ154"/>
+  <dimension ref="A1:FK154"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" style="104" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" style="27" customWidth="1" collapsed="1"/>
-    <col min="4" max="165" width="32" style="27" customWidth="1" collapsed="1"/>
-    <col min="166" max="16384" width="9.140625" style="27" collapsed="1"/>
+    <col min="2" max="3" width="39.28515625" style="104" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.7109375" style="27" customWidth="1" collapsed="1"/>
+    <col min="5" max="166" width="32" style="27" customWidth="1" collapsed="1"/>
+    <col min="167" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:166" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:167" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>156</v>
       </c>
       <c r="B1" s="85" t="s">
         <v>1688</v>
       </c>
-      <c r="C1" s="85">
+      <c r="C1" s="85" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D1" s="85">
         <v>2128</v>
       </c>
-      <c r="D1" s="13">
+      <c r="E1" s="13">
         <v>1259</v>
       </c>
-      <c r="E1" s="13">
+      <c r="F1" s="13">
         <v>1301</v>
       </c>
-      <c r="F1" s="13">
+      <c r="G1" s="13">
         <v>1309</v>
       </c>
-      <c r="G1" s="13">
+      <c r="H1" s="13">
         <v>1240</v>
       </c>
-      <c r="H1" s="13">
+      <c r="I1" s="13">
         <v>1315</v>
       </c>
-      <c r="I1" s="13">
+      <c r="J1" s="13">
         <v>1321</v>
       </c>
-      <c r="J1" s="13">
+      <c r="K1" s="13">
         <v>1216</v>
       </c>
-      <c r="K1" s="13">
+      <c r="L1" s="13">
         <v>1289</v>
       </c>
-      <c r="L1" s="13"/>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
@@ -16501,1343 +16530,1480 @@
       <c r="FG1" s="13"/>
       <c r="FH1" s="13"/>
       <c r="FI1" s="13"/>
-      <c r="FJ1" t="s">
+      <c r="FJ1" s="13"/>
+      <c r="FK1" t="s">
         <v>1094</v>
       </c>
     </row>
-    <row r="2" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
         <v>882</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="C2" s="102" t="s">
         <v>1619</v>
-      </c>
-      <c r="C2" s="106" t="s">
-        <v>1689</v>
       </c>
       <c r="D2" s="106" t="s">
         <v>1689</v>
       </c>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="106" t="s">
+        <v>1689</v>
+      </c>
+      <c r="F2" s="102" t="s">
         <v>1619</v>
       </c>
     </row>
-    <row r="3" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="102" t="s">
         <v>1256</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="C3" s="102" t="s">
         <v>1620</v>
-      </c>
-      <c r="C3" s="104" t="s">
-        <v>1690</v>
       </c>
       <c r="D3" s="104" t="s">
         <v>1690</v>
       </c>
-      <c r="E3" s="102" t="s">
+      <c r="E3" s="104" t="s">
+        <v>1690</v>
+      </c>
+      <c r="F3" s="102" t="s">
         <v>1620</v>
       </c>
     </row>
-    <row r="4" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="102" t="s">
         <v>1257</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="C4" s="102" t="s">
         <v>1621</v>
-      </c>
-      <c r="C4" s="106" t="s">
-        <v>1691</v>
       </c>
       <c r="D4" s="106" t="s">
         <v>1691</v>
       </c>
-      <c r="E4" s="102" t="s">
+      <c r="E4" s="106" t="s">
+        <v>1691</v>
+      </c>
+      <c r="F4" s="102" t="s">
         <v>1621</v>
       </c>
     </row>
-    <row r="5" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="102" t="s">
         <v>1258</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="C5" s="102" t="s">
         <v>1622</v>
-      </c>
-      <c r="C5" s="104" t="s">
-        <v>1692</v>
       </c>
       <c r="D5" s="104" t="s">
         <v>1692</v>
       </c>
-      <c r="E5" s="102" t="s">
+      <c r="E5" s="104" t="s">
+        <v>1692</v>
+      </c>
+      <c r="F5" s="102" t="s">
         <v>1622</v>
       </c>
     </row>
-    <row r="6" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="102" t="s">
         <v>1259</v>
       </c>
-      <c r="B6" s="102" t="s">
+      <c r="C6" s="102" t="s">
         <v>1623</v>
-      </c>
-      <c r="C6" s="106" t="s">
-        <v>1693</v>
       </c>
       <c r="D6" s="106" t="s">
         <v>1693</v>
       </c>
-      <c r="E6" s="102" t="s">
+      <c r="E6" s="106" t="s">
+        <v>1693</v>
+      </c>
+      <c r="F6" s="102" t="s">
         <v>1623</v>
       </c>
     </row>
-    <row r="7" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="102" t="s">
         <v>1260</v>
       </c>
-      <c r="B7" s="102" t="s">
+      <c r="C7" s="102" t="s">
         <v>1624</v>
-      </c>
-      <c r="C7" s="104" t="s">
-        <v>1694</v>
       </c>
       <c r="D7" s="104" t="s">
         <v>1694</v>
       </c>
-      <c r="E7" s="102" t="s">
+      <c r="E7" s="104" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F7" s="102" t="s">
         <v>1624</v>
       </c>
     </row>
-    <row r="8" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="102" t="s">
         <v>1261</v>
       </c>
-      <c r="B8" s="102" t="s">
+      <c r="C8" s="102" t="s">
         <v>215</v>
-      </c>
-      <c r="C8" s="104" t="s">
-        <v>611</v>
       </c>
       <c r="D8" s="104" t="s">
         <v>611</v>
       </c>
-      <c r="E8" s="102" t="s">
+      <c r="E8" s="104" t="s">
+        <v>611</v>
+      </c>
+      <c r="F8" s="102" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="102" t="s">
         <v>1262</v>
       </c>
-      <c r="C9" s="102" t="s">
+      <c r="D9" s="102" t="s">
         <v>1625</v>
       </c>
     </row>
-    <row r="10" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="102" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="102" t="s">
+      <c r="D10" s="102" t="s">
         <v>1626</v>
       </c>
     </row>
-    <row r="11" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="102" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="102" t="s">
+      <c r="D11" s="102" t="s">
         <v>1627</v>
       </c>
     </row>
-    <row r="12" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="102" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="102" t="s">
+      <c r="D12" s="102" t="s">
         <v>1628</v>
       </c>
     </row>
-    <row r="13" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="102" t="s">
         <v>1266</v>
       </c>
-      <c r="C13" s="102" t="s">
+      <c r="D13" s="102" t="s">
         <v>1629</v>
       </c>
     </row>
-    <row r="14" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="102" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="102" t="s">
+      <c r="D14" s="102" t="s">
         <v>1630</v>
       </c>
     </row>
-    <row r="15" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="102" t="s">
         <v>1268</v>
       </c>
-      <c r="C15" s="102" t="s">
+      <c r="D15" s="102" t="s">
         <v>1631</v>
       </c>
     </row>
-    <row r="16" spans="1:166" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:167" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="102" t="s">
         <v>1269</v>
       </c>
-      <c r="C16" s="102" t="s">
+      <c r="D16" s="102" t="s">
         <v>1632</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="102" t="s">
         <v>1270</v>
       </c>
-      <c r="C17" s="102" t="s">
+      <c r="D17" s="102" t="s">
         <v>1633</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="102" t="s">
         <v>1271</v>
       </c>
-      <c r="C18" s="102" t="s">
+      <c r="D18" s="102" t="s">
         <v>1459</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="102" t="s">
         <v>164</v>
       </c>
-      <c r="B19" t="s">
-        <v>1807</v>
-      </c>
-      <c r="C19" s="102" t="s">
+      <c r="B19">
+        <v>1009910</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1806</v>
+      </c>
+      <c r="D19" s="102" t="s">
         <v>1634</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="102" t="s">
         <v>1635</v>
       </c>
-      <c r="C20" s="102" t="s">
+      <c r="B20" s="102" t="s">
+        <v>1858</v>
+      </c>
+      <c r="D20" s="102" t="s">
         <v>1636</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="102" t="s">
         <v>1272</v>
       </c>
-      <c r="C21" s="102" t="s">
+      <c r="B21" s="102" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="102" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="102" t="s">
         <v>1452</v>
       </c>
-      <c r="C22" s="102" t="s">
+      <c r="B22" s="102">
+        <v>1007849</v>
+      </c>
+      <c r="D22" s="102" t="s">
         <v>1637</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="102" t="s">
         <v>1453</v>
       </c>
-      <c r="C23" s="102" t="s">
+      <c r="B23" s="102" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D23" s="102" t="s">
         <v>1638</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>159</v>
       </c>
-      <c r="B24" s="105" t="s">
+      <c r="B24" s="102"/>
+      <c r="C24" s="105" t="s">
         <v>987</v>
       </c>
-      <c r="C24" s="102" t="s">
+      <c r="D24" s="102" t="s">
         <v>1696</v>
       </c>
-      <c r="D24" s="102" t="s">
+      <c r="E24" s="102" t="s">
         <v>1695</v>
       </c>
-      <c r="E24" s="102" t="s">
+      <c r="F24" s="102" t="s">
         <v>1696</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1275</v>
       </c>
       <c r="B25" s="102"/>
-      <c r="C25" s="102" t="s">
-        <v>1530</v>
-      </c>
+      <c r="C25" s="102"/>
       <c r="D25" s="102" t="s">
         <v>1530</v>
       </c>
       <c r="E25" s="102" t="s">
         <v>1530</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="102" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1276</v>
       </c>
       <c r="B26" s="102"/>
-      <c r="C26" s="102" t="s">
+      <c r="C26" s="102"/>
+      <c r="D26" s="102" t="s">
         <v>1696</v>
       </c>
-      <c r="E26" s="102" t="s">
+      <c r="F26" s="102" t="s">
         <v>1696</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1277</v>
       </c>
       <c r="B27" s="102"/>
-      <c r="C27" s="102" t="s">
+      <c r="C27" s="102"/>
+      <c r="D27" s="102" t="s">
         <v>174</v>
       </c>
-      <c r="E27" s="102" t="s">
+      <c r="F27" s="102" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1278</v>
       </c>
       <c r="B28" s="102"/>
-      <c r="C28" t="s">
+      <c r="C28" s="102"/>
+      <c r="D28" t="s">
         <v>1714</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1279</v>
       </c>
       <c r="B29" s="102"/>
-      <c r="C29" t="s">
+      <c r="C29" s="102"/>
+      <c r="D29" t="s">
         <v>1714</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1282</v>
       </c>
       <c r="B30" s="102"/>
       <c r="C30" s="102"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="102"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1283</v>
       </c>
       <c r="B31" s="102"/>
-      <c r="C31" t="s">
+      <c r="C31" s="102"/>
+      <c r="D31" t="s">
         <v>1666</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1284</v>
       </c>
       <c r="B32" s="102"/>
-      <c r="C32" t="s">
+      <c r="C32" s="102"/>
+      <c r="D32" t="s">
         <v>1617</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1285</v>
       </c>
       <c r="B33" s="102"/>
-      <c r="C33" t="s">
+      <c r="C33" s="102"/>
+      <c r="D33" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1286</v>
       </c>
       <c r="B34" s="102"/>
-      <c r="C34" t="s">
+      <c r="C34" s="102"/>
+      <c r="D34" t="s">
         <v>1730</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>172</v>
       </c>
       <c r="B35" s="102"/>
-      <c r="C35" t="s">
+      <c r="C35" s="102"/>
+      <c r="D35" t="s">
         <v>1725</v>
       </c>
-      <c r="D35" s="102"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="102"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>207</v>
       </c>
       <c r="B36" s="102"/>
-      <c r="C36"/>
-      <c r="D36" s="102"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="102"/>
+      <c r="D36"/>
+      <c r="E36" s="102"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>960</v>
       </c>
       <c r="B37" s="102"/>
-      <c r="C37" t="s">
+      <c r="C37" s="102"/>
+      <c r="D37" t="s">
         <v>1717</v>
       </c>
-      <c r="D37" s="102"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="102"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1287</v>
       </c>
       <c r="B38" s="102"/>
-      <c r="C38" t="s">
+      <c r="C38" s="102"/>
+      <c r="D38" t="s">
         <v>1530</v>
       </c>
-      <c r="D38" s="102"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="102"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1288</v>
       </c>
       <c r="B39" s="102"/>
-      <c r="C39" t="s">
+      <c r="C39" s="102"/>
+      <c r="D39" t="s">
         <v>1717</v>
       </c>
-      <c r="D39" s="102"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="102"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1289</v>
       </c>
       <c r="B40" s="102"/>
-      <c r="C40" t="s">
+      <c r="C40" s="102"/>
+      <c r="D40" t="s">
         <v>174</v>
       </c>
-      <c r="D40" s="102"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="102"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="102" t="s">
         <v>1290</v>
       </c>
       <c r="B41" s="102"/>
-      <c r="C41" s="102" t="s">
+      <c r="C41" s="102"/>
+      <c r="D41" s="102" t="s">
         <v>1717</v>
       </c>
-      <c r="D41" s="102"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="102"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1291</v>
       </c>
       <c r="B42" s="102"/>
-      <c r="C42" t="s">
+      <c r="C42" s="102"/>
+      <c r="D42" t="s">
         <v>1719</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1292</v>
       </c>
       <c r="B43" s="102"/>
-      <c r="C43" t="s">
+      <c r="C43" s="102"/>
+      <c r="D43" t="s">
         <v>1719</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1293</v>
       </c>
       <c r="B44" s="102"/>
-      <c r="C44" t="s">
+      <c r="C44" s="102"/>
+      <c r="D44" t="s">
         <v>1719</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1294</v>
       </c>
       <c r="B45" s="102"/>
-      <c r="C45" t="s">
+      <c r="C45" s="102"/>
+      <c r="D45" t="s">
         <v>1717</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1295</v>
       </c>
       <c r="B46" s="102"/>
-      <c r="C46" t="s">
+      <c r="C46" s="102"/>
+      <c r="D46" t="s">
         <v>1720</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1296</v>
       </c>
       <c r="B47" s="102"/>
-      <c r="C47" t="s">
+      <c r="C47" s="102"/>
+      <c r="D47" t="s">
         <v>1720</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1297</v>
       </c>
       <c r="B48" s="102"/>
-      <c r="C48" s="105" t="s">
+      <c r="C48" s="102"/>
+      <c r="D48" s="105" t="s">
         <v>1718</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1298</v>
       </c>
       <c r="B49" s="102"/>
-      <c r="C49" s="102" t="s">
+      <c r="C49" s="102"/>
+      <c r="D49" s="102" t="s">
         <v>1530</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1299</v>
       </c>
       <c r="B50" s="102"/>
-      <c r="C50" s="105" t="s">
+      <c r="C50" s="102"/>
+      <c r="D50" s="105" t="s">
         <v>1718</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1300</v>
       </c>
       <c r="B51" s="102"/>
-      <c r="C51" s="102" t="s">
+      <c r="C51" s="102"/>
+      <c r="D51" s="102" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="102" t="s">
         <v>1301</v>
       </c>
       <c r="B52" s="102"/>
-      <c r="C52" s="105" t="s">
+      <c r="C52" s="102"/>
+      <c r="D52" s="105" t="s">
         <v>1718</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1302</v>
       </c>
       <c r="B53" s="102"/>
-      <c r="C53" t="s">
+      <c r="C53" s="102"/>
+      <c r="D53" t="s">
         <v>1721</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1303</v>
       </c>
       <c r="B54" s="102"/>
-      <c r="C54" t="s">
+      <c r="C54" s="102"/>
+      <c r="D54" t="s">
         <v>1721</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1304</v>
       </c>
       <c r="B55" s="102"/>
-      <c r="C55" t="s">
+      <c r="C55" s="102"/>
+      <c r="D55" t="s">
         <v>1720</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1305</v>
       </c>
       <c r="B56" s="102"/>
-      <c r="C56" t="s">
+      <c r="C56" s="102"/>
+      <c r="D56" t="s">
         <v>1717</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1306</v>
       </c>
       <c r="B57" s="102"/>
-      <c r="C57" t="s">
+      <c r="C57" s="102"/>
+      <c r="D57" t="s">
         <v>1721</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1307</v>
       </c>
       <c r="B58" s="102"/>
-      <c r="C58" t="s">
+      <c r="C58" s="102"/>
+      <c r="D58" t="s">
         <v>1718</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="102" t="s">
         <v>1316</v>
       </c>
       <c r="B59" s="102"/>
-      <c r="C59" s="104" t="s">
+      <c r="C59" s="102"/>
+      <c r="D59" s="104" t="s">
         <v>1765</v>
       </c>
-      <c r="D59" s="27" t="s">
+      <c r="E59" s="27" t="s">
         <v>1765</v>
       </c>
-      <c r="E59" s="102" t="s">
+      <c r="F59" s="102" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="102" t="s">
         <v>1317</v>
       </c>
       <c r="B60" s="102"/>
-      <c r="C60" s="105" t="s">
+      <c r="C60" s="102"/>
+      <c r="D60" s="105" t="s">
         <v>1734</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="102" t="s">
         <v>1318</v>
       </c>
       <c r="B61" s="102"/>
-      <c r="C61" s="105" t="s">
+      <c r="C61" s="102"/>
+      <c r="D61" s="105" t="s">
         <v>1700</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="102" t="s">
         <v>1319</v>
       </c>
       <c r="B62" s="102"/>
-      <c r="C62" s="105" t="s">
+      <c r="C62" s="102"/>
+      <c r="D62" s="105" t="s">
         <v>1733</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="102" t="s">
         <v>652</v>
       </c>
       <c r="B63" s="102"/>
-      <c r="C63" s="105" t="s">
+      <c r="C63" s="102"/>
+      <c r="D63" s="105" t="s">
         <v>1732</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="102" t="s">
         <v>1320</v>
       </c>
       <c r="B64" s="102"/>
-      <c r="C64" t="s">
+      <c r="C64" s="102"/>
+      <c r="D64" t="s">
         <v>1767</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1321</v>
       </c>
       <c r="B65" s="102"/>
-      <c r="C65" t="s">
+      <c r="C65" s="102"/>
+      <c r="D65" t="s">
         <v>1733</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1325</v>
       </c>
       <c r="B66" s="102"/>
       <c r="C66" s="102"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="102"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1326</v>
       </c>
       <c r="B67" s="102"/>
       <c r="C67" s="102"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="102"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1327</v>
       </c>
       <c r="B68" s="102"/>
       <c r="C68" s="102"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="102"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1328</v>
       </c>
       <c r="B69" s="102"/>
       <c r="C69" s="102"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="102"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1329</v>
       </c>
       <c r="B70" s="102"/>
       <c r="C70" s="102"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="102"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1330</v>
       </c>
       <c r="B71" s="102"/>
       <c r="C71" s="102"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="102"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1331</v>
       </c>
       <c r="B72" s="102"/>
       <c r="C72" s="102"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="102"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1332</v>
       </c>
       <c r="B73" s="102"/>
       <c r="C73" s="102"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="102"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1333</v>
       </c>
       <c r="B74" s="102"/>
       <c r="C74" s="102"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="102"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1335</v>
       </c>
       <c r="B75" s="102"/>
       <c r="C75" s="102"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="102"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1359</v>
       </c>
       <c r="B76" s="102"/>
-      <c r="C76" t="s">
+      <c r="C76" s="102"/>
+      <c r="D76" t="s">
         <v>1744</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="104" t="s">
         <v>1365</v>
       </c>
-      <c r="B77" s="106" t="s">
+      <c r="C77" s="106" t="s">
         <v>1695</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>1696</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="27" t="s">
         <v>1366</v>
       </c>
-      <c r="B78" s="106" t="s">
+      <c r="C78" s="106" t="s">
         <v>1789</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>1746</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1367</v>
       </c>
       <c r="B79" s="102"/>
-      <c r="C79" s="106"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="102"/>
+      <c r="D79" s="106"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1368</v>
       </c>
       <c r="B80" s="102"/>
-      <c r="C80" s="106"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="102"/>
+      <c r="D80" s="106"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1369</v>
       </c>
       <c r="B81" s="102"/>
-      <c r="C81" s="106"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="102"/>
+      <c r="D81" s="106"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1370</v>
       </c>
       <c r="B82" s="102"/>
-      <c r="C82" s="106"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="102"/>
+      <c r="D82" s="106"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1371</v>
       </c>
       <c r="B83" s="102"/>
-      <c r="C83" s="106"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="102"/>
+      <c r="D83" s="106"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1372</v>
       </c>
       <c r="B84" s="102"/>
-      <c r="C84" s="106"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="102"/>
+      <c r="D84" s="106"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1373</v>
       </c>
       <c r="B85" s="102"/>
-      <c r="C85"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="102"/>
+      <c r="D85"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1374</v>
       </c>
       <c r="B86" s="102"/>
-      <c r="C86"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="102"/>
+      <c r="D86"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1375</v>
       </c>
       <c r="B87" s="102"/>
-      <c r="C87"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="102"/>
+      <c r="D87"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1376</v>
       </c>
       <c r="B88" s="102"/>
-      <c r="C88"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="102"/>
+      <c r="D88"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1377</v>
       </c>
       <c r="B89" s="102"/>
-      <c r="C89"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="102"/>
+      <c r="D89"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1380</v>
       </c>
       <c r="B90" s="102"/>
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="102"/>
+      <c r="D90"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1381</v>
       </c>
       <c r="B91" s="102"/>
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="102"/>
+      <c r="D91"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1382</v>
       </c>
       <c r="B92" s="102"/>
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="102"/>
+      <c r="D92"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1383</v>
       </c>
       <c r="B93" s="102"/>
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="102"/>
+      <c r="D93"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1384</v>
       </c>
       <c r="B94" s="102"/>
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="102"/>
+      <c r="D94"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1385</v>
       </c>
       <c r="B95" s="102"/>
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="102"/>
+      <c r="D95"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1386</v>
       </c>
       <c r="B96" s="102"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C96" s="102"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1387</v>
       </c>
       <c r="B97" s="102"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C97" s="102"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1388</v>
       </c>
       <c r="B98" s="102"/>
-      <c r="C98" t="s">
+      <c r="C98" s="102"/>
+      <c r="D98" t="s">
         <v>1745</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1389</v>
       </c>
       <c r="B99" s="102"/>
-      <c r="C99" s="106"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="102"/>
+      <c r="D99" s="106"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1390</v>
       </c>
       <c r="B100" s="102"/>
-      <c r="C100" s="106"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C100" s="102"/>
+      <c r="D100" s="106"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="104" t="s">
         <v>1391</v>
       </c>
-      <c r="C101" s="106" t="s">
+      <c r="D101" s="106" t="s">
         <v>1724</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="104" t="s">
         <v>1392</v>
       </c>
-      <c r="C102" s="102" t="s">
+      <c r="D102" s="102" t="s">
         <v>1717</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="27" t="s">
         <v>1393</v>
       </c>
-      <c r="C103" s="106" t="s">
+      <c r="D103" s="106" t="s">
         <v>1724</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1397</v>
       </c>
       <c r="B104" s="102"/>
-      <c r="C104"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C104" s="102"/>
+      <c r="D104"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1399</v>
       </c>
       <c r="B105" s="102"/>
-      <c r="C105"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C105" s="102"/>
+      <c r="D105"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1400</v>
       </c>
       <c r="B106" s="102"/>
-      <c r="C106"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C106" s="102"/>
+      <c r="D106"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1401</v>
       </c>
       <c r="B107" s="102"/>
-      <c r="C107"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C107" s="102"/>
+      <c r="D107"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="102" t="s">
         <v>1402</v>
       </c>
       <c r="B108" s="102"/>
-      <c r="C108"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C108" s="102"/>
+      <c r="D108"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1403</v>
       </c>
       <c r="B109" s="102"/>
-      <c r="D109"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C109" s="102"/>
+      <c r="E109"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1404</v>
       </c>
       <c r="B110" s="102"/>
-      <c r="D110"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C110" s="102"/>
+      <c r="E110"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1405</v>
       </c>
       <c r="B111" s="102"/>
-      <c r="C111" t="s">
+      <c r="C111" s="102"/>
+      <c r="D111" t="s">
         <v>1749</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1406</v>
       </c>
       <c r="B112" s="102"/>
-      <c r="C112" t="s">
+      <c r="C112" s="102"/>
+      <c r="D112" t="s">
         <v>1724</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>1407</v>
       </c>
       <c r="B113" s="102"/>
-      <c r="C113" t="s">
+      <c r="C113" s="102"/>
+      <c r="D113" t="s">
         <v>1717</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>1408</v>
       </c>
       <c r="B114" s="102"/>
-      <c r="C114" t="s">
+      <c r="C114" s="102"/>
+      <c r="D114" t="s">
         <v>1751</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>1409</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="102"/>
+      <c r="C115" t="s">
         <v>1790</v>
       </c>
-      <c r="C115"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D115"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>1410</v>
       </c>
       <c r="B116" s="102"/>
-      <c r="C116"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C116" s="102"/>
+      <c r="D116"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>1411</v>
       </c>
       <c r="B117" s="102"/>
-      <c r="C117"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="102"/>
+      <c r="D117"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="104" t="s">
         <v>1412</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="104" t="s">
         <v>1413</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>1414</v>
       </c>
       <c r="B120" s="102"/>
-      <c r="C120" t="s">
+      <c r="C120" s="102"/>
+      <c r="D120" t="s">
         <v>1754</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>1439</v>
       </c>
       <c r="B121" s="102"/>
-      <c r="C121" t="s">
+      <c r="C121" s="102"/>
+      <c r="D121" t="s">
         <v>1759</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>1440</v>
       </c>
       <c r="B122" s="102"/>
-      <c r="C122" t="s">
+      <c r="C122" s="102"/>
+      <c r="D122" t="s">
         <v>1760</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>1441</v>
       </c>
       <c r="B123" s="102"/>
-      <c r="C123" t="s">
+      <c r="C123" s="102"/>
+      <c r="D123" t="s">
         <v>1761</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="27" t="s">
         <v>1442</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>1443</v>
       </c>
       <c r="B125" s="102"/>
-      <c r="C125" t="s">
+      <c r="C125" s="102"/>
+      <c r="D125" t="s">
         <v>1729</v>
       </c>
-      <c r="D125" s="102" t="s">
+      <c r="E125" s="102" t="s">
         <v>1729</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>1445</v>
       </c>
       <c r="B126" s="102"/>
-      <c r="C126" t="s">
+      <c r="C126" s="102"/>
+      <c r="D126" t="s">
         <v>1747</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>1446</v>
       </c>
       <c r="B127" s="102"/>
-      <c r="C127" t="s">
+      <c r="C127" s="102"/>
+      <c r="D127" t="s">
         <v>1748</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>1447</v>
       </c>
       <c r="B128" s="102"/>
-      <c r="C128" t="s">
+      <c r="C128" s="102"/>
+      <c r="D128" t="s">
         <v>1696</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>1448</v>
       </c>
       <c r="B129" s="102"/>
-      <c r="C129" t="s">
+      <c r="C129" s="102"/>
+      <c r="D129" t="s">
         <v>1766</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>1449</v>
       </c>
       <c r="B130" s="102"/>
-      <c r="C130" t="s">
+      <c r="C130" s="102"/>
+      <c r="D130" t="s">
         <v>1039</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>1450</v>
       </c>
       <c r="B131" s="102"/>
-      <c r="C131"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C131" s="102"/>
+      <c r="D131"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>1451</v>
       </c>
       <c r="B132" s="102"/>
-      <c r="C132" t="s">
+      <c r="C132" s="102"/>
+      <c r="D132" t="s">
         <v>1768</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>1452</v>
       </c>
       <c r="B133" s="102"/>
-      <c r="C133"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C133" s="102"/>
+      <c r="D133"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>1453</v>
       </c>
       <c r="B134" s="102"/>
-      <c r="C134"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C134" s="102"/>
+      <c r="D134"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>1456</v>
       </c>
       <c r="B135" s="102"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C135" s="102"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>1462</v>
       </c>
       <c r="B136" s="102"/>
-      <c r="C136"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C136" s="102"/>
+      <c r="D136"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>1468</v>
       </c>
       <c r="B137" s="102"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C137" s="102"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>1469</v>
       </c>
       <c r="B138" s="102"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C138" s="102"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>161</v>
       </c>
       <c r="B139" s="102"/>
-      <c r="C139"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C139" s="102"/>
+      <c r="D139"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="27" t="s">
         <v>1496</v>
       </c>
-      <c r="C140" s="102"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D140" s="102"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>1561</v>
       </c>
       <c r="B141" s="102"/>
-      <c r="C141" t="s">
+      <c r="C141" s="102"/>
+      <c r="D141" t="s">
         <v>1697</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>1569</v>
       </c>
       <c r="B142" s="102"/>
-      <c r="C142"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C142" s="102"/>
+      <c r="D142"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>1591</v>
       </c>
       <c r="B143" s="102"/>
-      <c r="C143"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C143" s="102"/>
+      <c r="D143"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="27" t="s">
         <v>1442</v>
       </c>
-      <c r="C144" s="27" t="s">
+      <c r="D144" s="27" t="s">
         <v>1763</v>
       </c>
-      <c r="H144" s="27" t="s">
+      <c r="I144" s="27" t="s">
         <v>1762</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="102" t="s">
         <v>1777</v>
       </c>
       <c r="B145" s="102"/>
-      <c r="C145" s="106" t="s">
+      <c r="C145" s="102"/>
+      <c r="D145" s="106" t="s">
         <v>1788</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="102" t="s">
         <v>1778</v>
       </c>
       <c r="B146" s="102"/>
-      <c r="C146" s="106" t="s">
+      <c r="C146" s="102"/>
+      <c r="D146" s="106" t="s">
         <v>1788</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="102" t="s">
         <v>1779</v>
       </c>
       <c r="B147" s="102"/>
-      <c r="C147" s="106" t="s">
+      <c r="C147" s="102"/>
+      <c r="D147" s="106" t="s">
         <v>1788</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="102" t="s">
         <v>1780</v>
       </c>
       <c r="B148" s="102"/>
-      <c r="C148" s="106" t="s">
+      <c r="C148" s="102"/>
+      <c r="D148" s="106" t="s">
         <v>1788</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="102" t="s">
         <v>1781</v>
       </c>
       <c r="B149" s="102"/>
-      <c r="C149" s="106" t="s">
+      <c r="C149" s="102"/>
+      <c r="D149" s="106" t="s">
         <v>1788</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="102" t="s">
         <v>1782</v>
       </c>
       <c r="B150" s="102"/>
-      <c r="C150" s="106" t="s">
+      <c r="C150" s="102"/>
+      <c r="D150" s="106" t="s">
         <v>1787</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="102" t="s">
         <v>1783</v>
       </c>
       <c r="B151" s="102"/>
-      <c r="C151" s="106" t="s">
+      <c r="C151" s="102"/>
+      <c r="D151" s="106" t="s">
         <v>1787</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="102" t="s">
         <v>1784</v>
       </c>
       <c r="B152" s="102"/>
-      <c r="C152" s="106" t="s">
+      <c r="C152" s="102"/>
+      <c r="D152" s="106" t="s">
         <v>1787</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="102" t="s">
         <v>1785</v>
       </c>
       <c r="B153" s="102"/>
-      <c r="C153" s="106" t="s">
+      <c r="C153" s="102"/>
+      <c r="D153" s="106" t="s">
         <v>1787</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="102" t="s">
         <v>1786</v>
       </c>
       <c r="B154" s="102"/>
-      <c r="C154" s="106" t="s">
+      <c r="C154" s="102"/>
+      <c r="D154" s="106" t="s">
         <v>1787</v>
       </c>
     </row>
@@ -17848,7 +18014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -18231,7 +18397,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -18307,7 +18473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -18350,7 +18516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18390,7 +18556,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:BN3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18814,7 +18980,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -19145,11 +19311,11 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:AQ6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6:AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19797,7 +19963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19882,7 +20048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -20212,7 +20378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:AQ6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20713,7 +20879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -21895,7 +22061,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21980,7 +22146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -22302,7 +22468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22862,7 +23028,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22930,7 +23096,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
@@ -23265,7 +23431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23825,7 +23991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23899,7 +24065,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24234,7 +24400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24794,7 +24960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24868,7 +25034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -26922,7 +27088,7 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27257,7 +27423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27817,7 +27983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27891,7 +28057,7 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27955,7 +28121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28029,7 +28195,7 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28104,7 +28270,7 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28179,7 +28345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28255,7 +28421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28317,7 +28483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28379,7 +28545,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -28624,7 +28790,7 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -28854,7 +29020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -28897,7 +29063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -28943,7 +29109,7 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -29001,7 +29167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -29301,7 +29467,7 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -29365,7 +29531,7 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -29435,7 +29601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -29987,12 +30153,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
-    <hyperlink ref="C8" r:id="rId2"/>
-    <hyperlink ref="D8" r:id="rId3"/>
-    <hyperlink ref="E8" r:id="rId4"/>
-    <hyperlink ref="F8" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-3800-000000000000}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{00000000-0004-0000-3800-000001000000}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-3800-000002000000}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{00000000-0004-0000-3800-000003000000}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{00000000-0004-0000-3800-000004000000}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-3800-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -30000,7 +30166,7 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -30166,10 +30332,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="1307AutomationUser@sudler.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="1307AutomationUser@sudler.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="1307AutomationUser@sudler.com"/>
-    <hyperlink ref="E2" r:id="rId4" display="1307AutomationUser@sudler.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="1307AutomationUser@sudler.com" xr:uid="{00000000-0004-0000-3900-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" display="1307AutomationUser@sudler.com" xr:uid="{00000000-0004-0000-3900-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" display="1307AutomationUser@sudler.com" xr:uid="{00000000-0004-0000-3900-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" display="1307AutomationUser@sudler.com" xr:uid="{00000000-0004-0000-3900-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -30177,7 +30343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -30569,8 +30735,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
-    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-3A00-000000000000}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{00000000-0004-0000-3A00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -30578,7 +30744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -30745,7 +30911,7 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -30803,7 +30969,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="1307TestEmployeeAutomation1234@gmail.com"/>
+    <hyperlink ref="B8" r:id="rId1" display="1307TestEmployeeAutomation1234@gmail.com" xr:uid="{00000000-0004-0000-3B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -30811,7 +30977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -30879,7 +31045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -31230,7 +31396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -31451,7 +31617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -31512,7 +31678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -31573,7 +31739,7 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -31796,7 +31962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -32038,7 +32204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -32096,7 +32262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -32340,7 +32506,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -32417,7 +32583,7 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -32475,7 +32641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -32731,7 +32897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -32789,7 +32955,7 @@
 </file>
 
 <file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -33031,7 +33197,7 @@
 </file>
 
 <file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -33273,7 +33439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -33331,7 +33497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -33389,7 +33555,7 @@
 </file>
 
 <file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -33575,7 +33741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4D00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -33706,7 +33872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -33837,7 +34003,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -33898,7 +34064,7 @@
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -34014,7 +34180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -34134,7 +34300,7 @@
 </file>
 
 <file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5100-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -34277,7 +34443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5200-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -34319,7 +34485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5300-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -34367,7 +34533,7 @@
 </file>
 
 <file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5400-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -34426,7 +34592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5500-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -34516,7 +34682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5600-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -34669,7 +34835,7 @@
 </file>
 
 <file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5700-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -34820,7 +34986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5800-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -34924,7 +35090,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -35051,7 +35217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5900-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -35108,7 +35274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5A00-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -35172,7 +35338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5B00-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -35278,7 +35444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5C00-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -35335,7 +35501,7 @@
 </file>
 
 <file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5D00-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -35399,7 +35565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5E00-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -35491,7 +35657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5F00-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -35547,7 +35713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6000-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -35644,7 +35810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6100-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -35770,7 +35936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6200-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>

</xml_diff>